<commit_message>
Telegram Scheduler in python
</commit_message>
<xml_diff>
--- a/logs/messages.xlsx
+++ b/logs/messages.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -928,6 +928,622 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Post 5.jpg</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>5</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>👫🏻 **Celebrate the unbreakable bond of sibling love**
+⚡ 50%-80% off
+👉🏻 amzaff.to/93m1fy6
+🎁 **Person</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2025-07-21 12:18:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Post 3.jpg</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>3</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🧶 **amazonkarigar | Threads of heritage**
+👉🏻 amzaff.to/otM7QCn
+🔥 **Latest Arrivals** 🔥
+🚩 **Indian </t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>2025-07-21 12:22:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Post 1.jpg</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>🔥 **BLOCKBUSTER DEALS OF THE DAY** 🔥
+💰 **Prime Everyday Savings**
+⚡ Up to 60% off
++ Extra 5% off,
+-</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>2025-07-21 12:22:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Post 4.jpg</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>4</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>📺 **Smart TVs &amp; Projectors**
+⚡ Starting at ₹8,999
+👉🏻 amzaff.to/Kkk481A
+⏱️ **Limited Time Mega Deals</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>2025-07-21 12:22:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Post 5.jpg</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>5</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>👫🏻 **Celebrate the unbreakable bond of sibling love**
+⚡ 50%-80% off
+👉🏻 amzaff.to/93m1fy6
+🎁 **Person</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>2025-07-21 12:23:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Post 2.jpg</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>2</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>💥 **Mega Electronic Days**
+📣 Sale live till 20th July
+💻 **Laptops, Smartwatches, Headphones &amp; more*</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>2025-07-21 12:24:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Post 1.jpg</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>🔥 **BLOCKBUSTER DEALS OF THE DAY** 🔥
+💰 **Prime Everyday Savings**
+⚡ Up to 60% off
++ Extra 5% off,
+-</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>2025-07-21 12:24:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Post 3.jpg</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>3</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🧶 **amazonkarigar | Threads of heritage**
+👉🏻 amzaff.to/otM7QCn
+🔥 **Latest Arrivals** 🔥
+🚩 **Indian </t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>2025-07-21 12:24:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Post 4.jpg</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>4</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>📺 **Smart TVs &amp; Projectors**
+⚡ Starting at ₹8,999
+👉🏻 amzaff.to/Kkk481A
+⏱️ **Limited Time Mega Deals</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>2025-07-21 12:24:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Post 5.jpg</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>5</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>👫🏻 **Celebrate the unbreakable bond of sibling love**
+⚡ 50%-80% off
+👉🏻 amzaff.to/93m1fy6
+🎁 **Person</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>2025-07-21 12:24:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Post 2.jpg</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>2</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>💥 **Mega Electronic Days**
+📣 Sale live till 20th July
+💻 **Laptops, Smartwatches, Headphones &amp; more*</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>2025-07-21 12:32:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Post 3.jpg</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>3</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🧶 **amazonkarigar | Threads of heritage**
+👉🏻 amzaff.to/otM7QCn
+🔥 **Latest Arrivals** 🔥
+🚩 **Indian </t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>2025-07-21 12:36:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Post 2.jpg</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>2</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>💥 **Mega Electronic Days**
+📣 Sale live till 20th July
+💻 **Laptops, Smartwatches, Headphones &amp; more*</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>2025-07-21 12:38:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Post 1.jpg</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>🔥 **BLOCKBUSTER DEALS OF THE DAY** 🔥
+💰 **Prime Everyday Savings**
+⚡ Up to 60% off
++ Extra 5% off,
+-</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>2025-07-21 12:38:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Post 4.jpg</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>4</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>📺 **Smart TVs &amp; Projectors**
+⚡ Starting at ₹8,999
+👉🏻 amzaff.to/Kkk481A
+⏱️ **Limited Time Mega Deals</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>2025-07-21 12:38:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Post 3.jpg</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>3</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🧶 **amazonkarigar | Threads of heritage**
+👉🏻 amzaff.to/otM7QCn
+🔥 **Latest Arrivals** 🔥
+🚩 **Indian </t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>2025-07-21 12:38:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Post 5.jpg</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>5</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>👫🏻 **Celebrate the unbreakable bond of sibling love**
+⚡ 50%-80% off
+👉🏻 amzaff.to/93m1fy6
+🎁 **Person</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>2025-07-21 12:38:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Post 2.jpg</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>2</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>💥 **Mega Electronic Days**
+📣 Sale live till 20th July
+💻 **Laptops, Smartwatches, Headphones &amp; more*</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>2025-07-21 12:40:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Post 1.jpg</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>🔥 **BLOCKBUSTER DEALS OF THE DAY** 🔥
+💰 **Prime Everyday Savings**
+⚡ Up to 60% off
++ Extra 5% off,
+-</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>2025-07-21 12:40:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Post 3.jpg</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>3</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🧶 **amazonkarigar | Threads of heritage**
+👉🏻 amzaff.to/otM7QCn
+🔥 **Latest Arrivals** 🔥
+🚩 **Indian </t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>2025-07-21 12:40:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Post 4.jpg</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>4</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>📺 **Smart TVs &amp; Projectors**
+⚡ Starting at ₹8,999
+👉🏻 amzaff.to/Kkk481A
+⏱️ **Limited Time Mega Deals</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>2025-07-21 12:40:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Post 5.jpg</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>5</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>👫🏻 **Celebrate the unbreakable bond of sibling love**
+⚡ 50%-80% off
+👉🏻 amzaff.to/93m1fy6
+🎁 **Person</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>2025-07-21 12:40:10</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Auto scheduler partially done
</commit_message>
<xml_diff>
--- a/logs/messages.xlsx
+++ b/logs/messages.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:F104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,11 @@
           <t>timestamp</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>category</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -487,6 +492,7 @@
           <t>2025-07-17 16:23:03</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -515,6 +521,7 @@
           <t>2025-07-17 16:23:07</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -543,6 +550,7 @@
           <t>2025-07-17 16:23:13</t>
         </is>
       </c>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -571,6 +579,7 @@
           <t>2025-07-17 16:27:03</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -599,6 +608,7 @@
           <t>2025-07-17 16:27:07</t>
         </is>
       </c>
+      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -620,6 +630,7 @@
           <t>2025-07-17 16:27:13</t>
         </is>
       </c>
+      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -648,6 +659,7 @@
           <t>2025-07-17 16:30:07</t>
         </is>
       </c>
+      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -669,6 +681,7 @@
           <t>2025-07-17 16:30:13</t>
         </is>
       </c>
+      <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -697,6 +710,7 @@
           <t>2025-07-17 18:24:04</t>
         </is>
       </c>
+      <c r="F10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -725,6 +739,7 @@
           <t>2025-07-17 18:25:02</t>
         </is>
       </c>
+      <c r="F11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -746,6 +761,7 @@
           <t>2025-07-17 18:26:03</t>
         </is>
       </c>
+      <c r="F12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -774,6 +790,7 @@
           <t>2025-07-17 19:49:04</t>
         </is>
       </c>
+      <c r="F13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -802,6 +819,7 @@
           <t>2025-07-17 19:49:04</t>
         </is>
       </c>
+      <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -823,6 +841,7 @@
           <t>2025-07-17 19:49:05</t>
         </is>
       </c>
+      <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -851,6 +870,7 @@
           <t>2025-07-17 19:50:05</t>
         </is>
       </c>
+      <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -872,6 +892,7 @@
           <t>2025-07-17 19:50:05</t>
         </is>
       </c>
+      <c r="F17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -900,6 +921,7 @@
           <t>2025-07-17 19:50:05</t>
         </is>
       </c>
+      <c r="F18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -927,6 +949,7 @@
           <t>2025-07-18 12:38:03</t>
         </is>
       </c>
+      <c r="F19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -955,6 +978,7 @@
           <t>2025-07-21 12:18:04</t>
         </is>
       </c>
+      <c r="F20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -983,6 +1007,7 @@
           <t>2025-07-21 12:22:05</t>
         </is>
       </c>
+      <c r="F21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1012,6 +1037,7 @@
           <t>2025-07-21 12:22:05</t>
         </is>
       </c>
+      <c r="F22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1040,6 +1066,7 @@
           <t>2025-07-21 12:22:06</t>
         </is>
       </c>
+      <c r="F23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1068,6 +1095,7 @@
           <t>2025-07-21 12:23:05</t>
         </is>
       </c>
+      <c r="F24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1095,6 +1123,7 @@
           <t>2025-07-21 12:24:12</t>
         </is>
       </c>
+      <c r="F25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1124,6 +1153,7 @@
           <t>2025-07-21 12:24:14</t>
         </is>
       </c>
+      <c r="F26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1152,6 +1182,7 @@
           <t>2025-07-21 12:24:14</t>
         </is>
       </c>
+      <c r="F27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1180,6 +1211,7 @@
           <t>2025-07-21 12:24:14</t>
         </is>
       </c>
+      <c r="F28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1208,6 +1240,7 @@
           <t>2025-07-21 12:24:14</t>
         </is>
       </c>
+      <c r="F29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1235,6 +1268,7 @@
           <t>2025-07-21 12:32:25</t>
         </is>
       </c>
+      <c r="F30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1263,6 +1297,7 @@
           <t>2025-07-21 12:36:03</t>
         </is>
       </c>
+      <c r="F31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1290,6 +1325,7 @@
           <t>2025-07-21 12:38:08</t>
         </is>
       </c>
+      <c r="F32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1319,6 +1355,7 @@
           <t>2025-07-21 12:38:09</t>
         </is>
       </c>
+      <c r="F33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1347,6 +1384,7 @@
           <t>2025-07-21 12:38:09</t>
         </is>
       </c>
+      <c r="F34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1375,6 +1413,7 @@
           <t>2025-07-21 12:38:10</t>
         </is>
       </c>
+      <c r="F35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1403,6 +1442,7 @@
           <t>2025-07-21 12:38:10</t>
         </is>
       </c>
+      <c r="F36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1430,6 +1470,7 @@
           <t>2025-07-21 12:40:09</t>
         </is>
       </c>
+      <c r="F37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1459,6 +1500,7 @@
           <t>2025-07-21 12:40:10</t>
         </is>
       </c>
+      <c r="F38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1487,6 +1529,7 @@
           <t>2025-07-21 12:40:10</t>
         </is>
       </c>
+      <c r="F39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1515,6 +1558,7 @@
           <t>2025-07-21 12:40:10</t>
         </is>
       </c>
+      <c r="F40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1543,6 +1587,7 @@
           <t>2025-07-21 12:40:10</t>
         </is>
       </c>
+      <c r="F41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr"/>
@@ -1568,6 +1613,7 @@
           <t>2025-07-21 16:55:00</t>
         </is>
       </c>
+      <c r="F42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr"/>
@@ -1593,6 +1639,7 @@
           <t>2025-07-21 16:56:00</t>
         </is>
       </c>
+      <c r="F43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr"/>
@@ -1618,6 +1665,7 @@
           <t>2025-07-21 16:59:01</t>
         </is>
       </c>
+      <c r="F44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr"/>
@@ -1643,6 +1691,7 @@
           <t>2025-07-21 17:01:00</t>
         </is>
       </c>
+      <c r="F45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr"/>
@@ -1668,6 +1717,7 @@
           <t>2025-07-21 18:15:00</t>
         </is>
       </c>
+      <c r="F46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr"/>
@@ -1693,6 +1743,7 @@
           <t>2025-07-21 18:20:01</t>
         </is>
       </c>
+      <c r="F47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr"/>
@@ -1718,6 +1769,7 @@
           <t>2025-07-21 18:24:01</t>
         </is>
       </c>
+      <c r="F48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr"/>
@@ -1743,6 +1795,7 @@
           <t>2025-07-21 18:25:03</t>
         </is>
       </c>
+      <c r="F49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr"/>
@@ -1768,6 +1821,7 @@
           <t>2025-07-21 18:27:01</t>
         </is>
       </c>
+      <c r="F50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr"/>
@@ -1793,6 +1847,7 @@
           <t>2025-07-21 18:30:00</t>
         </is>
       </c>
+      <c r="F51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr"/>
@@ -1818,6 +1873,7 @@
           <t>2025-07-21 18:32:00</t>
         </is>
       </c>
+      <c r="F52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr"/>
@@ -1843,6 +1899,7 @@
           <t>2025-07-21 18:37:00</t>
         </is>
       </c>
+      <c r="F53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1872,6 +1929,7 @@
           <t>2025-07-21 18:39:03</t>
         </is>
       </c>
+      <c r="F54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1900,6 +1958,1417 @@
           <t>2025-07-21 19:31:03</t>
         </is>
       </c>
+      <c r="F55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Post 1.jpg</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>1</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>🔥**BLOCKBUSTER DEALS OF THE DAY** 🔥 
+🎧  **Mobile Accessories Days**
+⚡  Up to 70% off
+📣  Last day of</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>2025-07-21 20:19:03</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Post 1.jpg</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>1</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>🔥**BLOCKBUSTER DEALS OF THE DAY** 🔥 
+🎧  **Mobile Accessories Days**
+⚡  Up to 70% off
+📣  Last day of</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>2025-07-21 20:22:02</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Post 1.jpg</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>1</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>TIMING : 
+10:30 AM
+🔥 **BLOCKBUSTER DEALS OF THE DAY** 🔥
+💰 **Prime Everyday Savings**
+⚡ Up to 60% of</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>2025-07-22 10:34:04</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Post 1.jpg</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>1</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>TIMING : 
+10:30 AM
+🔥 **BLOCKBUSTER DEALS OF THE DAY** 🔥
+💰 **Prime Everyday Savings**
+⚡ Up to 60% of</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>2025-07-23 10:52:03</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Post 2.jpg</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>2</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>💥 **Mega Electronic Days**
+📣 Sale live till 20th July
+💻 **Laptops, Smartwatches, Headphones &amp; more*</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>2025-07-23 10:53:03</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Post 3.jpg</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>3</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🧶 **amazonkarigar | Threads of heritage**
+👉🏻 amzaff.to/otM7QCn
+🔥 **Latest Arrivals** 🔥
+🚩 **Indian </t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>2025-07-23 10:54:03</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Post 4.jpg</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>4</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>📺 **Smart TVs &amp; Projectors**
+⚡ Starting at ₹8,999
+👉🏻 amzaff.to/Kkk481A
+⏱️ **Limited Time Mega Deals</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>2025-07-23 10:55:04</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Post 1.jpg</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>1</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>TIMING : 
+10:30 AM
+🔥 **BLOCKBUSTER DEALS OF THE DAY** 🔥
+💰 **Prime Everyday Savings**
+⚡ Up to 60% of</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>2025-07-23 10:56:08</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Post 2.jpg</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>2</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>💥 **Mega Electronic Days**
+📣 Sale live till 20th July
+💻 **Laptops, Smartwatches, Headphones &amp; more*</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>2025-07-23 10:56:32</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Post 1.jpg</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>1</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>TIMING : 
+10:30 AM
+🔥 **BLOCKBUSTER DEALS OF THE DAY** 🔥
+💰 **Prime Everyday Savings**
+⚡ Up to 60% of</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>2025-07-23 11:00:06</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Post 2.jpg</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>2</v>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>💥 **Mega Electronic Days**
+📣 Sale live till 20th July
+💻 **Laptops, Smartwatches, Headphones &amp; more*</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>2025-07-23 11:01:03</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Post 1.jpg</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>1</v>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>TIMING : 
+10:30 AM
+🔥 **BLOCKBUSTER DEALS OF THE DAY** 🔥
+💰 **Prime Everyday Savings**
+⚡ Up to 60% of</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>2025-07-23 11:10:04</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Post 2.jpg</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>2</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>💥 **Mega Electronic Days**
+📣 Sale live till 20th July
+💻 **Laptops, Smartwatches, Headphones &amp; more*</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Image + Text sent</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>2025-07-23 11:11:04</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr"/>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Post 1.jpg</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>1</v>
+      </c>
+      <c r="C69" t="inlineStr"/>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Image only sent</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>2025-07-23 14:27:06</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr"/>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>post-1.jpg</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>1</v>
+      </c>
+      <c r="C70" t="inlineStr"/>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Image only sent</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>2025-07-24 14:43:03</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr"/>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>post-2.jpg</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>1</v>
+      </c>
+      <c r="C71" t="inlineStr"/>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Image only sent</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>2025-07-24 14:44:32</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr"/>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>post-1.jpg</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>1</v>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>🔥 **BLOCKBUSTER DEALS OF THE DAY** 🔥
+💥 Price Crash Store
+⚡️ Up to 5% off
+👉🏻 amzaff.in/l3swo0g
+🌟 Ki</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Image + Text sent (split)</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>2025-07-24 19:50:06</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr"/>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>post-2.jpg</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>1</v>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t xml:space="preserve">💧 **Everyday Essentials for Skin, Hair &amp; Fragrance** 💧
+💥 Maximise earnings with Beauty commissions </t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Image + Text sent (split)</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>2025-07-24 19:51:03</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr"/>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr"/>
+      <c r="B74" t="n">
+        <v>1</v>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>💻 **Entry Level Gaming Laptops**
+⚡️ Up to 45% off
+👉🏻 amzaff.in/FeVABNi
+🔥 Gaming Laptops Under ₹80,0</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Text only sent (split if needed)</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>2025-07-24 19:52:00</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr"/>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>post1.jpg</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>1</v>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>🔥 **BLOCKBUSTER DEALS OF THE DAY** 🔥
+💥 Price Crash Store
+⚡️ Up to 5% off
+👉🏻 amzaff.in/l3swo0g
+🌟 Ki</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Image + Text sent (split)</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>2025-07-25 10:57:01</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr"/>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>post2.jpg</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>1</v>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">💧 **Everyday Essentials for Skin, Hair &amp; Fragrance** 💧
+💥 Maximise earnings with Beauty commissions </t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Image + Text sent (split)</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>2025-07-25 10:58:01</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr"/>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr"/>
+      <c r="B77" t="n">
+        <v>1</v>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>💻 **Entry Level Gaming Laptops**
+⚡️ Up to 45% off
+👉🏻 amzaff.in/FeVABNi
+🔥 Gaming Laptops Under ₹80,0</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Text only sent (split if needed)</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>2025-07-25 10:59:00</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr"/>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>post-1.jpg</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>1</v>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>🔥 **BLOCKBUSTER DEALS OF THE DAY** 🔥
+💥 Price Crash Store
+⚡️ Up to 5% off
+👉🏻 amzaff.in/l3swo0g
+🌟 Ki</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Image + Text sent (split)</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>2025-07-25 14:10:02</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr"/>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>post-2.jpg</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>1</v>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">💧 **Everyday Essentials for Skin, Hair &amp; Fragrance** 💧
+💥 Maximise earnings with Beauty commissions </t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Image + Text sent (split)</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>2025-07-25 14:11:02</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr"/>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr"/>
+      <c r="B80" t="n">
+        <v>1</v>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>💻 **Entry Level Gaming Laptops**
+⚡️ Up to 45% off
+👉🏻 amzaff.in/FeVABNi
+🔥 Gaming Laptops Under ₹80,0</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Text only sent (split if needed)</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>2025-07-25 14:12:00</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr"/>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>post1.jpg</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>1</v>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>🔥 **BLOCKBUSTER DEALS OF THE DAY** 🔥
+💥 Price Crash Store
+⚡️ Up to 5% off
+👉🏻 amzaff.in/l3swo0g
+🌟 Ki</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Image + Text sent (split)</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>2025-07-25 14:15:00</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr"/>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>post2.jpg</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>1</v>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t xml:space="preserve">💧 **Everyday Essentials for Skin, Hair &amp; Fragrance** 💧
+💥 Maximise earnings with Beauty commissions </t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Image + Text sent (split)</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>2025-07-25 14:16:00</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr"/>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr"/>
+      <c r="B83" t="n">
+        <v>1</v>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>💻 **Entry Level Gaming Laptops**
+⚡️ Up to 45% off
+👉🏻 amzaff.in/FeVABNi
+🔥 Gaming Laptops Under ₹80,0</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Text only sent (split if needed)</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>2025-07-25 14:17:00</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr"/>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>post2.jpg</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>1</v>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t xml:space="preserve">💧 **Everyday Essentials for Skin, Hair &amp; Fragrance** 💧
+💥 Maximise earnings with Beauty commissions </t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Image + Text sent (split)</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>2025-07-25 14:18:20</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr"/>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr"/>
+      <c r="B85" t="n">
+        <v>1</v>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>💻 **Entry Level Gaming Laptops**
+⚡️ Up to 45% off
+👉🏻 amzaff.in/FeVABNi
+🔥 Gaming Laptops Under ₹80,0</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Text only sent (split if needed)</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>2025-07-25 14:21:40</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr"/>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>post1.jpg</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>1</v>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>🔥 **BLOCKBUSTER DEALS OF THE DAY** 🔥
+💥 Price Crash Store
+⚡️ Up to 5% off
+👉🏻 amzaff.in/l3swo0g
+🌟 Ki</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Image + Text sent (split)</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>2025-07-25 16:10:00</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr"/>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>post2.jpg</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>1</v>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t xml:space="preserve">💧 **Everyday Essentials for Skin, Hair &amp; Fragrance** 💧
+💥 Maximise earnings with Beauty commissions </t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Image + Text sent (split)</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>2025-07-25 16:13:20</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr"/>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr"/>
+      <c r="B88" t="n">
+        <v>1</v>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>💻 **Entry Level Gaming Laptops**
+⚡️ Up to 45% off
+👉🏻 amzaff.in/FeVABNi
+🔥 Gaming Laptops Under ₹80,0</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Text only sent (split if needed)</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>2025-07-25 16:16:40</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr"/>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>post-1.jpg</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>1</v>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>🔥 **BLOCKBUSTER DEALS OF THE DAY** 🔥
+💥 Price Crash Store
+⚡️ Up to 5% off
+👉🏻 amzaff.in/l3swo0g
+🌟 Ki</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Image + Text sent (split)</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>2025-07-26 17:45:06</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>Kid's Carnival</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr"/>
+      <c r="B90" t="n">
+        <v>2</v>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t xml:space="preserve">💧 **Everyday Essentials for Skin, Hair &amp; Fragrance** 💧
+💥 Maximise earnings with Beauty commissions </t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Text only sent (split if needed)</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>2025-07-26 17:48:20</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>Daily Essentials</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>post-3.jpg</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>3</v>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>💻 **Entry Level Gaming Laptops**
+⚡️ Up to 45% off
+👉🏻 amzaff.in/FeVABNi
+🔥 Gaming Laptops Under ₹80,0</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Image + Text sent (split)</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>2025-07-26 17:51:44</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>Laptops</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>post-1.jpg</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>1</v>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>🔥 **BLOCKBUSTER DEALS OF THE DAY** 🔥
+💥 Price Crash Store
+⚡️ Up to 5% off
+👉🏻 amzaff.in/l3swo0g
+🌟 Ki</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Scheduled Image + Text at None</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>2025-07-26 18:15:07</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>Kid's Carnival</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr"/>
+      <c r="B93" t="n">
+        <v>2</v>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t xml:space="preserve">💧 **Everyday Essentials for Skin, Hair &amp; Fragrance** 💧
+💥 Maximise earnings with Beauty commissions </t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Scheduled Text only at None</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>2025-07-26 18:18:20</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>Daily Essentials</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>post-3.jpg</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>3</v>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>💻 **Entry Level Gaming Laptops**
+⚡️ Up to 45% off
+👉🏻 amzaff.in/FeVABNi
+🔥 Gaming Laptops Under ₹80,0</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Scheduled Image + Text at None</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>2025-07-26 18:21:43</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>Laptops</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>post-1.jpg</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>1</v>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>🔥 **BLOCKBUSTER DEALS OF THE DAY** 🔥
+💥 Price Crash Store
+⚡️ Up to 5% off
+👉🏻 amzaff.in/l3swo0g
+🌟 Ki</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Scheduled Image + Text at None</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>2025-07-26 18:30:06</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>Kid's Carnival</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr"/>
+      <c r="B96" t="n">
+        <v>2</v>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t xml:space="preserve">💧 **Everyday Essentials for Skin, Hair &amp; Fragrance** 💧
+💥 Maximise earnings with Beauty commissions </t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Scheduled Text only at None</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>2025-07-26 18:35:00</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>Daily Essentials</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>post-3.jpg</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>3</v>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>💻 **Entry Level Gaming Laptops**
+⚡️ Up to 45% off
+👉🏻 amzaff.in/FeVABNi
+🔥 Gaming Laptops Under ₹80,0</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Scheduled Image + Text at None</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>2025-07-26 18:40:04</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>Laptops</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>post1.jpg</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>1</v>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>🔥 **BLOCKBUSTER DEALS OF THE DAY** 🔥
+💥 Price Crash Store
+⚡️ Up to 5% off
+👉🏻 amzaff.in/l3swo0g
+🌟 Ki</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Scheduled Image + Text at None</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>2025-07-26 19:05:03</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>Kid's Carnival</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>post2.jpg</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>2</v>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t xml:space="preserve">💧 **Everyday Essentials for Skin, Hair &amp; Fragrance** 💧
+💥 Maximise earnings with Beauty commissions </t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Scheduled Image + Text at None</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>2025-07-26 19:10:01</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>Daily Essentials</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr"/>
+      <c r="B100" t="n">
+        <v>3</v>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>💻 **Entry Level Gaming Laptops**
+⚡️ Up to 45% off
+👉🏻 amzaff.in/FeVABNi
+🔥 Gaming Laptops Under ₹80,0</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Scheduled Text only at None</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>2025-07-26 19:15:00</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>Laptops</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>post-1.jpg</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>1</v>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>🔥 **BLOCKBUSTER DEALS OF THE DAY** 🔥
+💥 Price Crash Store
+⚡️ Up to 5% off
+👉🏻 amzaff.in/l3swo0g
+🌟 Ki</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>Scheduled Image + Text at None</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>2025-07-26 19:40:03</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>Kid's Carnival</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>post-1.jpg</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>1</v>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>🔥 **BLOCKBUSTER DEALS OF THE DAY** 🔥
+💥 Price Crash Store
+⚡️ Up to 5% off
+👉🏻 amzaff.in/l3swo0g
+🌟 Ki</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>Scheduled Image + Text at None</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>2025-07-26 20:00:06</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>Kid's Carnival</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr"/>
+      <c r="B103" t="n">
+        <v>2</v>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">💧 **Everyday Essentials for Skin, Hair &amp; Fragrance** 💧
+💥 Maximise earnings with Beauty commissions </t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Scheduled Text only at None</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>2025-07-26 20:02:30</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>Daily Essentials</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>post-3.jpg</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>3</v>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>💻 **Entry Level Gaming Laptops**
+⚡️ Up to 45% off
+👉🏻 amzaff.in/FeVABNi
+🔥 Gaming Laptops Under ₹80,0</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Scheduled Image + Text at None</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>2025-07-26 20:05:03</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>Laptops</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>